<commit_message>
continuation of the same work at home
</commit_message>
<xml_diff>
--- a/data/results_fft_morph_depth.xlsx
+++ b/data/results_fft_morph_depth.xlsx
@@ -502,10 +502,10 @@
         <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.5925125641246545</v>
+        <v>0.5297855048019494</v>
       </c>
       <c r="I2" t="n">
-        <v>0.08095470060839145</v>
+        <v>0.05306360429042664</v>
       </c>
     </row>
     <row r="3">
@@ -535,10 +535,10 @@
         <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>1.128625900413797</v>
+        <v>0.9975627310283326</v>
       </c>
       <c r="I3" t="n">
-        <v>0.1313725850210809</v>
+        <v>0.1155566321558266</v>
       </c>
     </row>
     <row r="4">
@@ -568,10 +568,10 @@
         <v>1</v>
       </c>
       <c r="H4" t="n">
-        <v>1.151077593651681</v>
+        <v>1.065315069088294</v>
       </c>
       <c r="I4" t="n">
-        <v>0.06588101835710128</v>
+        <v>0.1427956937476589</v>
       </c>
     </row>
     <row r="5">
@@ -601,10 +601,10 @@
         <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.7582475820206624</v>
+        <v>0.7470287814537109</v>
       </c>
       <c r="I5" t="n">
-        <v>0.1063406659490936</v>
+        <v>0.1677466073687303</v>
       </c>
     </row>
     <row r="6">
@@ -634,10 +634,10 @@
         <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6755469056709107</v>
+        <v>0.7171265693569835</v>
       </c>
       <c r="I6" t="n">
-        <v>0.218901380866883</v>
+        <v>0.2515030733153356</v>
       </c>
     </row>
     <row r="7">
@@ -667,10 +667,10 @@
         <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.7421887084619248</v>
+        <v>0.8166802768446795</v>
       </c>
       <c r="I7" t="n">
-        <v>0.225722728155242</v>
+        <v>0.257224835533526</v>
       </c>
     </row>
     <row r="8">
@@ -700,10 +700,10 @@
         <v>1</v>
       </c>
       <c r="H8" t="n">
-        <v>0.7577933498394818</v>
+        <v>0.8688388354752572</v>
       </c>
       <c r="I8" t="n">
-        <v>0.2868399592795025</v>
+        <v>0.2954030563117702</v>
       </c>
     </row>
   </sheetData>

</xml_diff>